<commit_message>
implementing some final fixes in graphics and sound. ready
</commit_message>
<xml_diff>
--- a/V1/matlab/data/song1.xlsx
+++ b/V1/matlab/data/song1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d75c386ba75b0d57/Documents/Prog/PianoHero/V1/matlab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\OneDrive\Documents\Prog\PianoHero\V1\matlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E8FFA59-BA70-4276-B7B8-075BD869BB09}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="8_{8E8FFA59-BA70-4276-B7B8-075BD869BB09}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{D13E2C09-1041-490E-85C3-95955EB58935}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="6980" xr2:uid="{8320D160-4322-4E27-BDF8-3F3E01AFB8DC}"/>
   </bookViews>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78BC464-DBA2-4B1E-866E-D1818F04B37B}">
-  <dimension ref="B2:N42"/>
+  <dimension ref="B2:N87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -466,1647 +466,3516 @@
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>200</v>
+        <v>-15</v>
       </c>
       <c r="C3">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D3">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E3">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F3">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="G3">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H3">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I3">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J3">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K3">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L3">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M3">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N3">
-        <v>-50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="C4">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D4">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E4">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F4">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G4">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="H4">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I4">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J4">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K4">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L4">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M4">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="N4">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="C5">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D5">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E5">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F5">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="G5">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H5">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I5">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J5">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K5">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="L5">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M5">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N5">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="C6">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="E6">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F6">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G6">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H6">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I6">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="J6">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K6">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L6">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M6">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N6">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="C7">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D7">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E7">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F7">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G7">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H7">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I7">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J7">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K7">
-        <v>200</v>
+        <v>-15</v>
       </c>
       <c r="L7">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M7">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N7">
-        <v>-50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C8">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D8">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E8">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F8">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G8">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H8">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I8">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="J8">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="L8">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M8">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="N8">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C9">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D9">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E9">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F9">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G9">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="H9">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I9">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J9">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L9">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M9">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N9">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C10">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D10">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E10">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F10">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="G10">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H10">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I10">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="J10">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="L10">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M10">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N10">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C11">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D11">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="E11">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F11">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G11">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H11">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I11">
-        <v>200</v>
+        <v>-15</v>
       </c>
       <c r="J11">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K11">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L11">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M11">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N11">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="C12">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D12">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E12">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F12">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G12">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H12">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="J12">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K12">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L12">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M12">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="N12">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C13">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D13">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E13">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F13">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G13">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H13">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="J13">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K13">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="L13">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M13">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="N13">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B14">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C14">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D14">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E14">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F14">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G14">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H14">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J14">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K14">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="L14">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M14">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N14">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B15">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C15">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D15">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E15">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F15">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G15">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H15">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I15">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="J15">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K15">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L15">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M15">
-        <v>200</v>
+        <v>-15</v>
       </c>
       <c r="N15">
-        <v>-50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B16">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C16">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D16">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E16">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F16">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G16">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="H16">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I16">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J16">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K16">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L16">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="N16">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B17">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="C17">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D17">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E17">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F17">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="G17">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H17">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I17">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J17">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K17">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L17">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="N17">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B18">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C18">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D18">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="E18">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F18">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G18">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H18">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I18">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J18">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K18">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L18">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M18">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="N18">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B19">
-        <v>200</v>
+        <v>-15</v>
       </c>
       <c r="C19">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D19">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E19">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F19">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="G19">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="H19">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I19">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J19">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K19">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L19">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M19">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N19">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B20">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="C20">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D20">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E20">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F20">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="G20">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H20">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I20">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J20">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K20">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L20">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M20">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N20">
-        <v>50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B21">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="C21">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D21">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="E21">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F21">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G21">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H21">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I21">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J21">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K21">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L21">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M21">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="N21">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B22">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C22">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D22">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E22">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F22">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G22">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H22">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I22">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J22">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K22">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L22">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M22">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N22">
-        <v>50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B23">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C23">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D23">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E23">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F23">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="G23">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="H23">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I23">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J23">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K23">
-        <v>200</v>
+        <v>-15</v>
       </c>
       <c r="L23">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M23">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N23">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B24">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C24">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D24">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E24">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F24">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="G24">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H24">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I24">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J24">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="L24">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M24">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N24">
-        <v>50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B25">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C25">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D25">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="E25">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F25">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G25">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H25">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I25">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J25">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="L25">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M25">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="N25">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B26">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="C26">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D26">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E26">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F26">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G26">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H26">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I26">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J26">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="L26">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M26">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N26">
-        <v>50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B27">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C27">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D27">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E27">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F27">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G27">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="H27">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I27">
-        <v>200</v>
+        <v>-15</v>
       </c>
       <c r="J27">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K27">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L27">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M27">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N27">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B28">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C28">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D28">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E28">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F28">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="G28">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="H28">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="J28">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K28">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L28">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M28">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N28">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B29">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C29">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D29">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="E29">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F29">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="G29">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H29">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="J29">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K29">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L29">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M29">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N29">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B30">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="C30">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D30">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="E30">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F30">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G30">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H30">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="J30">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K30">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L30">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M30">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N30">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B31">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C31">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D31">
-        <v>95</v>
+        <v>-15</v>
       </c>
       <c r="E31">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F31">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G31">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="H31">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I31">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="J31">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K31">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L31">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M31">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N31">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B32">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C32">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D32">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="E32">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F32">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="G32">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H32">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I32">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J32">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K32">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L32">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M32">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N32">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B33">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C33">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D33">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="E33">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F33">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G33">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H33">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I33">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="J33">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K33">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L33">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M33">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N33">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B34">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="C34">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D34">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E34">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F34">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G34">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H34">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I34">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J34">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K34">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L34">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M34">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="N34">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B35">
-        <v>195</v>
+        <v>-15</v>
       </c>
       <c r="C35">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D35">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E35">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F35">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G35">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H35">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I35">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J35">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K35">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L35">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M35">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N35">
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B36">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="C36">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D36">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E36">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F36">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G36">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H36">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I36">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J36">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K36">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="L36">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M36">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="N36">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B37">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="C37">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D37">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E37">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F37">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G37">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H37">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I37">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="J37">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K37">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="L37">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M37">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N37">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B38">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="C38">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D38">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E38">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F38">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="G38">
-        <v>50</v>
+        <v>-15</v>
       </c>
       <c r="H38">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I38">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="J38">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K38">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L38">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M38">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N38">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B39">
-        <v>200</v>
+        <v>-15</v>
       </c>
       <c r="C39">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D39">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E39">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F39">
-        <v>200</v>
+        <v>-15</v>
       </c>
       <c r="G39">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H39">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I39">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J39">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K39">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L39">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M39">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N39">
-        <v>-50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B40">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="C40">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D40">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E40">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="G40">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H40">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I40">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J40">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K40">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L40">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M40">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="N40">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B41">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="C41">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D41">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E41">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="G41">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H41">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I41">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="J41">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K41">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="L41">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M41">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N41">
-        <v>-50</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B42">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="C42">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="D42">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="E42">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="G42">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="H42">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="I42">
-        <v>-50</v>
+        <v>15</v>
       </c>
       <c r="J42">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="K42">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="L42">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="M42">
-        <v>-50</v>
+        <v>-15</v>
       </c>
       <c r="N42">
-        <v>-50</v>
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B43">
+        <v>-15</v>
+      </c>
+      <c r="C43">
+        <v>-15</v>
+      </c>
+      <c r="D43">
+        <v>-15</v>
+      </c>
+      <c r="E43">
+        <v>-15</v>
+      </c>
+      <c r="F43">
+        <v>-15</v>
+      </c>
+      <c r="G43">
+        <v>-15</v>
+      </c>
+      <c r="H43">
+        <v>-15</v>
+      </c>
+      <c r="I43">
+        <v>-15</v>
+      </c>
+      <c r="J43">
+        <v>-15</v>
+      </c>
+      <c r="K43">
+        <v>-15</v>
+      </c>
+      <c r="L43">
+        <v>-15</v>
+      </c>
+      <c r="M43">
+        <v>-15</v>
+      </c>
+      <c r="N43">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B44">
+        <v>-15</v>
+      </c>
+      <c r="C44">
+        <v>-15</v>
+      </c>
+      <c r="D44">
+        <v>-15</v>
+      </c>
+      <c r="E44">
+        <v>-15</v>
+      </c>
+      <c r="F44">
+        <v>-15</v>
+      </c>
+      <c r="G44">
+        <v>-15</v>
+      </c>
+      <c r="H44">
+        <v>-15</v>
+      </c>
+      <c r="I44">
+        <v>-15</v>
+      </c>
+      <c r="J44">
+        <v>-15</v>
+      </c>
+      <c r="K44">
+        <v>-15</v>
+      </c>
+      <c r="L44">
+        <v>-15</v>
+      </c>
+      <c r="M44">
+        <v>15</v>
+      </c>
+      <c r="N44">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B45">
+        <v>-15</v>
+      </c>
+      <c r="C45">
+        <v>-15</v>
+      </c>
+      <c r="D45">
+        <v>-15</v>
+      </c>
+      <c r="E45">
+        <v>-15</v>
+      </c>
+      <c r="F45">
+        <v>-15</v>
+      </c>
+      <c r="G45">
+        <v>-15</v>
+      </c>
+      <c r="H45">
+        <v>-15</v>
+      </c>
+      <c r="I45">
+        <v>-15</v>
+      </c>
+      <c r="J45">
+        <v>-15</v>
+      </c>
+      <c r="K45">
+        <v>15</v>
+      </c>
+      <c r="L45">
+        <v>-15</v>
+      </c>
+      <c r="M45">
+        <v>-15</v>
+      </c>
+      <c r="N45">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>-15</v>
+      </c>
+      <c r="C46">
+        <v>-15</v>
+      </c>
+      <c r="D46">
+        <v>-15</v>
+      </c>
+      <c r="E46">
+        <v>-15</v>
+      </c>
+      <c r="F46">
+        <v>-15</v>
+      </c>
+      <c r="G46">
+        <v>-15</v>
+      </c>
+      <c r="H46">
+        <v>-15</v>
+      </c>
+      <c r="I46">
+        <v>15</v>
+      </c>
+      <c r="J46">
+        <v>-15</v>
+      </c>
+      <c r="K46">
+        <v>-15</v>
+      </c>
+      <c r="L46">
+        <v>-15</v>
+      </c>
+      <c r="M46">
+        <v>-15</v>
+      </c>
+      <c r="N46">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <v>-15</v>
+      </c>
+      <c r="C47">
+        <v>-15</v>
+      </c>
+      <c r="D47">
+        <v>-15</v>
+      </c>
+      <c r="E47">
+        <v>-15</v>
+      </c>
+      <c r="F47">
+        <v>-15</v>
+      </c>
+      <c r="G47">
+        <v>-15</v>
+      </c>
+      <c r="H47">
+        <v>-15</v>
+      </c>
+      <c r="I47">
+        <v>-15</v>
+      </c>
+      <c r="J47">
+        <v>-15</v>
+      </c>
+      <c r="K47">
+        <v>-15</v>
+      </c>
+      <c r="L47">
+        <v>-15</v>
+      </c>
+      <c r="M47">
+        <v>-15</v>
+      </c>
+      <c r="N47">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B48">
+        <v>-15</v>
+      </c>
+      <c r="C48">
+        <v>-15</v>
+      </c>
+      <c r="D48">
+        <v>-15</v>
+      </c>
+      <c r="E48">
+        <v>-15</v>
+      </c>
+      <c r="F48">
+        <v>-15</v>
+      </c>
+      <c r="G48">
+        <v>-15</v>
+      </c>
+      <c r="H48">
+        <v>-15</v>
+      </c>
+      <c r="I48">
+        <v>-15</v>
+      </c>
+      <c r="J48">
+        <v>-15</v>
+      </c>
+      <c r="K48">
+        <v>-15</v>
+      </c>
+      <c r="L48">
+        <v>-15</v>
+      </c>
+      <c r="M48">
+        <v>-15</v>
+      </c>
+      <c r="N48">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B49">
+        <v>15</v>
+      </c>
+      <c r="C49">
+        <v>-15</v>
+      </c>
+      <c r="D49">
+        <v>-15</v>
+      </c>
+      <c r="E49">
+        <v>-15</v>
+      </c>
+      <c r="F49">
+        <v>-15</v>
+      </c>
+      <c r="G49">
+        <v>-15</v>
+      </c>
+      <c r="H49">
+        <v>-15</v>
+      </c>
+      <c r="I49">
+        <v>-15</v>
+      </c>
+      <c r="J49">
+        <v>-15</v>
+      </c>
+      <c r="K49">
+        <v>-15</v>
+      </c>
+      <c r="L49">
+        <v>-15</v>
+      </c>
+      <c r="M49">
+        <v>-15</v>
+      </c>
+      <c r="N49">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B50">
+        <v>-15</v>
+      </c>
+      <c r="C50">
+        <v>-15</v>
+      </c>
+      <c r="D50">
+        <v>-15</v>
+      </c>
+      <c r="E50">
+        <v>-15</v>
+      </c>
+      <c r="F50">
+        <v>-15</v>
+      </c>
+      <c r="G50">
+        <v>-15</v>
+      </c>
+      <c r="H50">
+        <v>-15</v>
+      </c>
+      <c r="I50">
+        <v>-15</v>
+      </c>
+      <c r="J50">
+        <v>-15</v>
+      </c>
+      <c r="K50">
+        <v>-15</v>
+      </c>
+      <c r="L50">
+        <v>-15</v>
+      </c>
+      <c r="M50">
+        <v>-15</v>
+      </c>
+      <c r="N50">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B51">
+        <v>-15</v>
+      </c>
+      <c r="C51">
+        <v>-15</v>
+      </c>
+      <c r="D51">
+        <v>15</v>
+      </c>
+      <c r="E51">
+        <v>-15</v>
+      </c>
+      <c r="F51">
+        <v>-15</v>
+      </c>
+      <c r="G51">
+        <v>-15</v>
+      </c>
+      <c r="H51">
+        <v>-15</v>
+      </c>
+      <c r="I51">
+        <v>-15</v>
+      </c>
+      <c r="J51">
+        <v>-15</v>
+      </c>
+      <c r="K51">
+        <v>-15</v>
+      </c>
+      <c r="L51">
+        <v>-15</v>
+      </c>
+      <c r="M51">
+        <v>-15</v>
+      </c>
+      <c r="N51">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B52">
+        <v>-15</v>
+      </c>
+      <c r="C52">
+        <v>-15</v>
+      </c>
+      <c r="D52">
+        <v>-15</v>
+      </c>
+      <c r="E52">
+        <v>-15</v>
+      </c>
+      <c r="F52">
+        <v>-15</v>
+      </c>
+      <c r="G52">
+        <v>15</v>
+      </c>
+      <c r="H52">
+        <v>-15</v>
+      </c>
+      <c r="I52">
+        <v>-15</v>
+      </c>
+      <c r="J52">
+        <v>-15</v>
+      </c>
+      <c r="K52">
+        <v>-15</v>
+      </c>
+      <c r="L52">
+        <v>-15</v>
+      </c>
+      <c r="M52">
+        <v>-15</v>
+      </c>
+      <c r="N52">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B53">
+        <v>-15</v>
+      </c>
+      <c r="C53">
+        <v>-15</v>
+      </c>
+      <c r="D53">
+        <v>-15</v>
+      </c>
+      <c r="E53">
+        <v>-15</v>
+      </c>
+      <c r="F53">
+        <v>15</v>
+      </c>
+      <c r="G53">
+        <v>-15</v>
+      </c>
+      <c r="H53">
+        <v>-15</v>
+      </c>
+      <c r="I53">
+        <v>-15</v>
+      </c>
+      <c r="J53">
+        <v>-15</v>
+      </c>
+      <c r="K53">
+        <v>-15</v>
+      </c>
+      <c r="L53">
+        <v>-15</v>
+      </c>
+      <c r="M53">
+        <v>-15</v>
+      </c>
+      <c r="N53">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B54">
+        <v>-15</v>
+      </c>
+      <c r="C54">
+        <v>-15</v>
+      </c>
+      <c r="D54">
+        <v>15</v>
+      </c>
+      <c r="E54">
+        <v>-15</v>
+      </c>
+      <c r="F54">
+        <v>-15</v>
+      </c>
+      <c r="G54">
+        <v>-15</v>
+      </c>
+      <c r="H54">
+        <v>-15</v>
+      </c>
+      <c r="I54">
+        <v>-15</v>
+      </c>
+      <c r="J54">
+        <v>-15</v>
+      </c>
+      <c r="K54">
+        <v>-15</v>
+      </c>
+      <c r="L54">
+        <v>-15</v>
+      </c>
+      <c r="M54">
+        <v>-15</v>
+      </c>
+      <c r="N54">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B55">
+        <v>-15</v>
+      </c>
+      <c r="C55">
+        <v>-15</v>
+      </c>
+      <c r="D55">
+        <v>-15</v>
+      </c>
+      <c r="E55">
+        <v>-15</v>
+      </c>
+      <c r="F55">
+        <v>-15</v>
+      </c>
+      <c r="G55">
+        <v>-15</v>
+      </c>
+      <c r="H55">
+        <v>-15</v>
+      </c>
+      <c r="I55">
+        <v>15</v>
+      </c>
+      <c r="J55">
+        <v>-15</v>
+      </c>
+      <c r="K55">
+        <v>-15</v>
+      </c>
+      <c r="L55">
+        <v>-15</v>
+      </c>
+      <c r="M55">
+        <v>-15</v>
+      </c>
+      <c r="N55">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B56">
+        <v>-15</v>
+      </c>
+      <c r="C56">
+        <v>-15</v>
+      </c>
+      <c r="D56">
+        <v>-15</v>
+      </c>
+      <c r="E56">
+        <v>-15</v>
+      </c>
+      <c r="F56">
+        <v>-15</v>
+      </c>
+      <c r="G56">
+        <v>-15</v>
+      </c>
+      <c r="H56">
+        <v>-15</v>
+      </c>
+      <c r="I56">
+        <v>-15</v>
+      </c>
+      <c r="J56">
+        <v>-15</v>
+      </c>
+      <c r="K56">
+        <v>-15</v>
+      </c>
+      <c r="L56">
+        <v>-15</v>
+      </c>
+      <c r="M56">
+        <v>-15</v>
+      </c>
+      <c r="N56">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B57">
+        <v>-15</v>
+      </c>
+      <c r="C57">
+        <v>-15</v>
+      </c>
+      <c r="D57">
+        <v>-15</v>
+      </c>
+      <c r="E57">
+        <v>-15</v>
+      </c>
+      <c r="F57">
+        <v>-15</v>
+      </c>
+      <c r="G57">
+        <v>-15</v>
+      </c>
+      <c r="H57">
+        <v>-15</v>
+      </c>
+      <c r="I57">
+        <v>15</v>
+      </c>
+      <c r="J57">
+        <v>-15</v>
+      </c>
+      <c r="K57">
+        <v>-15</v>
+      </c>
+      <c r="L57">
+        <v>-15</v>
+      </c>
+      <c r="M57">
+        <v>-15</v>
+      </c>
+      <c r="N57">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B58">
+        <v>-15</v>
+      </c>
+      <c r="C58">
+        <v>-15</v>
+      </c>
+      <c r="D58">
+        <v>-15</v>
+      </c>
+      <c r="E58">
+        <v>-15</v>
+      </c>
+      <c r="F58">
+        <v>-15</v>
+      </c>
+      <c r="G58">
+        <v>-15</v>
+      </c>
+      <c r="H58">
+        <v>-15</v>
+      </c>
+      <c r="I58">
+        <v>-15</v>
+      </c>
+      <c r="J58">
+        <v>-15</v>
+      </c>
+      <c r="K58">
+        <v>-15</v>
+      </c>
+      <c r="L58">
+        <v>-15</v>
+      </c>
+      <c r="M58">
+        <v>-15</v>
+      </c>
+      <c r="N58">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B59">
+        <v>-15</v>
+      </c>
+      <c r="C59">
+        <v>-15</v>
+      </c>
+      <c r="D59">
+        <v>-15</v>
+      </c>
+      <c r="E59">
+        <v>-15</v>
+      </c>
+      <c r="F59">
+        <v>-15</v>
+      </c>
+      <c r="G59">
+        <v>15</v>
+      </c>
+      <c r="H59">
+        <v>-15</v>
+      </c>
+      <c r="I59">
+        <v>-15</v>
+      </c>
+      <c r="J59">
+        <v>-15</v>
+      </c>
+      <c r="K59">
+        <v>-15</v>
+      </c>
+      <c r="L59">
+        <v>-15</v>
+      </c>
+      <c r="M59">
+        <v>-15</v>
+      </c>
+      <c r="N59">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B60">
+        <v>-15</v>
+      </c>
+      <c r="C60">
+        <v>-15</v>
+      </c>
+      <c r="D60">
+        <v>-15</v>
+      </c>
+      <c r="E60">
+        <v>-15</v>
+      </c>
+      <c r="F60">
+        <v>-15</v>
+      </c>
+      <c r="G60">
+        <v>-15</v>
+      </c>
+      <c r="H60">
+        <v>-15</v>
+      </c>
+      <c r="I60">
+        <v>15</v>
+      </c>
+      <c r="J60">
+        <v>-15</v>
+      </c>
+      <c r="K60">
+        <v>-15</v>
+      </c>
+      <c r="L60">
+        <v>-15</v>
+      </c>
+      <c r="M60">
+        <v>-15</v>
+      </c>
+      <c r="N60">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B61">
+        <v>-15</v>
+      </c>
+      <c r="C61">
+        <v>-15</v>
+      </c>
+      <c r="D61">
+        <v>-15</v>
+      </c>
+      <c r="E61">
+        <v>-15</v>
+      </c>
+      <c r="F61">
+        <v>-15</v>
+      </c>
+      <c r="G61">
+        <v>15</v>
+      </c>
+      <c r="H61">
+        <v>-15</v>
+      </c>
+      <c r="I61">
+        <v>-15</v>
+      </c>
+      <c r="J61">
+        <v>-15</v>
+      </c>
+      <c r="K61">
+        <v>-15</v>
+      </c>
+      <c r="L61">
+        <v>-15</v>
+      </c>
+      <c r="M61">
+        <v>-15</v>
+      </c>
+      <c r="N61">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B62">
+        <v>-15</v>
+      </c>
+      <c r="C62">
+        <v>-15</v>
+      </c>
+      <c r="D62">
+        <v>-15</v>
+      </c>
+      <c r="E62">
+        <v>-15</v>
+      </c>
+      <c r="F62">
+        <v>-15</v>
+      </c>
+      <c r="G62">
+        <v>-15</v>
+      </c>
+      <c r="H62">
+        <v>-15</v>
+      </c>
+      <c r="I62">
+        <v>15</v>
+      </c>
+      <c r="J62">
+        <v>-15</v>
+      </c>
+      <c r="K62">
+        <v>-15</v>
+      </c>
+      <c r="L62">
+        <v>-15</v>
+      </c>
+      <c r="M62">
+        <v>-15</v>
+      </c>
+      <c r="N62">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B63">
+        <v>-15</v>
+      </c>
+      <c r="C63">
+        <v>-15</v>
+      </c>
+      <c r="D63">
+        <v>-15</v>
+      </c>
+      <c r="E63">
+        <v>-15</v>
+      </c>
+      <c r="F63">
+        <v>-15</v>
+      </c>
+      <c r="G63">
+        <v>15</v>
+      </c>
+      <c r="H63">
+        <v>-15</v>
+      </c>
+      <c r="I63">
+        <v>-15</v>
+      </c>
+      <c r="J63">
+        <v>-15</v>
+      </c>
+      <c r="K63">
+        <v>-15</v>
+      </c>
+      <c r="L63">
+        <v>-15</v>
+      </c>
+      <c r="M63">
+        <v>-15</v>
+      </c>
+      <c r="N63">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B64">
+        <v>-15</v>
+      </c>
+      <c r="C64">
+        <v>-15</v>
+      </c>
+      <c r="D64">
+        <v>-15</v>
+      </c>
+      <c r="E64">
+        <v>-15</v>
+      </c>
+      <c r="F64">
+        <v>-15</v>
+      </c>
+      <c r="G64">
+        <v>-15</v>
+      </c>
+      <c r="H64">
+        <v>-15</v>
+      </c>
+      <c r="I64">
+        <v>15</v>
+      </c>
+      <c r="J64">
+        <v>-15</v>
+      </c>
+      <c r="K64">
+        <v>-15</v>
+      </c>
+      <c r="L64">
+        <v>-15</v>
+      </c>
+      <c r="M64">
+        <v>-15</v>
+      </c>
+      <c r="N64">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B65">
+        <v>-15</v>
+      </c>
+      <c r="C65">
+        <v>-15</v>
+      </c>
+      <c r="D65">
+        <v>-15</v>
+      </c>
+      <c r="E65">
+        <v>-15</v>
+      </c>
+      <c r="F65">
+        <v>-15</v>
+      </c>
+      <c r="G65">
+        <v>15</v>
+      </c>
+      <c r="H65">
+        <v>-15</v>
+      </c>
+      <c r="I65">
+        <v>-15</v>
+      </c>
+      <c r="J65">
+        <v>-15</v>
+      </c>
+      <c r="K65">
+        <v>-15</v>
+      </c>
+      <c r="L65">
+        <v>-15</v>
+      </c>
+      <c r="M65">
+        <v>-15</v>
+      </c>
+      <c r="N65">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="66" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B66">
+        <v>-15</v>
+      </c>
+      <c r="C66">
+        <v>-15</v>
+      </c>
+      <c r="D66">
+        <v>-15</v>
+      </c>
+      <c r="E66">
+        <v>-15</v>
+      </c>
+      <c r="F66">
+        <v>-15</v>
+      </c>
+      <c r="G66">
+        <v>-15</v>
+      </c>
+      <c r="H66">
+        <v>-15</v>
+      </c>
+      <c r="I66">
+        <v>15</v>
+      </c>
+      <c r="J66">
+        <v>-15</v>
+      </c>
+      <c r="K66">
+        <v>-15</v>
+      </c>
+      <c r="L66">
+        <v>-15</v>
+      </c>
+      <c r="M66">
+        <v>-15</v>
+      </c>
+      <c r="N66">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="67" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B67">
+        <v>-15</v>
+      </c>
+      <c r="C67">
+        <v>-15</v>
+      </c>
+      <c r="D67">
+        <v>-15</v>
+      </c>
+      <c r="E67">
+        <v>-15</v>
+      </c>
+      <c r="F67">
+        <v>15</v>
+      </c>
+      <c r="G67">
+        <v>-15</v>
+      </c>
+      <c r="H67">
+        <v>-15</v>
+      </c>
+      <c r="I67">
+        <v>-15</v>
+      </c>
+      <c r="J67">
+        <v>-15</v>
+      </c>
+      <c r="K67">
+        <v>-15</v>
+      </c>
+      <c r="L67">
+        <v>-15</v>
+      </c>
+      <c r="M67">
+        <v>-15</v>
+      </c>
+      <c r="N67">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="68" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B68">
+        <v>-15</v>
+      </c>
+      <c r="C68">
+        <v>-15</v>
+      </c>
+      <c r="D68">
+        <v>-15</v>
+      </c>
+      <c r="E68">
+        <v>-15</v>
+      </c>
+      <c r="F68">
+        <v>-15</v>
+      </c>
+      <c r="G68">
+        <v>-15</v>
+      </c>
+      <c r="H68">
+        <v>-15</v>
+      </c>
+      <c r="I68">
+        <v>15</v>
+      </c>
+      <c r="J68">
+        <v>-15</v>
+      </c>
+      <c r="K68">
+        <v>-15</v>
+      </c>
+      <c r="L68">
+        <v>-15</v>
+      </c>
+      <c r="M68">
+        <v>-15</v>
+      </c>
+      <c r="N68">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="69" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B69">
+        <v>-15</v>
+      </c>
+      <c r="C69">
+        <v>-15</v>
+      </c>
+      <c r="D69">
+        <v>-15</v>
+      </c>
+      <c r="E69">
+        <v>-15</v>
+      </c>
+      <c r="F69">
+        <v>15</v>
+      </c>
+      <c r="G69">
+        <v>-15</v>
+      </c>
+      <c r="H69">
+        <v>-15</v>
+      </c>
+      <c r="I69">
+        <v>-15</v>
+      </c>
+      <c r="J69">
+        <v>-15</v>
+      </c>
+      <c r="K69">
+        <v>-15</v>
+      </c>
+      <c r="L69">
+        <v>-15</v>
+      </c>
+      <c r="M69">
+        <v>-15</v>
+      </c>
+      <c r="N69">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="70" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B70">
+        <v>-15</v>
+      </c>
+      <c r="C70">
+        <v>-15</v>
+      </c>
+      <c r="D70">
+        <v>-15</v>
+      </c>
+      <c r="E70">
+        <v>-15</v>
+      </c>
+      <c r="F70">
+        <v>-15</v>
+      </c>
+      <c r="G70">
+        <v>-15</v>
+      </c>
+      <c r="H70">
+        <v>-15</v>
+      </c>
+      <c r="I70">
+        <v>15</v>
+      </c>
+      <c r="J70">
+        <v>-15</v>
+      </c>
+      <c r="K70">
+        <v>-15</v>
+      </c>
+      <c r="L70">
+        <v>-15</v>
+      </c>
+      <c r="M70">
+        <v>-15</v>
+      </c>
+      <c r="N70">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B71">
+        <v>-15</v>
+      </c>
+      <c r="C71">
+        <v>-15</v>
+      </c>
+      <c r="D71">
+        <v>-15</v>
+      </c>
+      <c r="E71">
+        <v>-15</v>
+      </c>
+      <c r="F71">
+        <v>15</v>
+      </c>
+      <c r="G71">
+        <v>-15</v>
+      </c>
+      <c r="H71">
+        <v>-15</v>
+      </c>
+      <c r="I71">
+        <v>-15</v>
+      </c>
+      <c r="J71">
+        <v>-15</v>
+      </c>
+      <c r="K71">
+        <v>-15</v>
+      </c>
+      <c r="L71">
+        <v>-15</v>
+      </c>
+      <c r="M71">
+        <v>-15</v>
+      </c>
+      <c r="N71">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="72" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B72">
+        <v>-15</v>
+      </c>
+      <c r="C72">
+        <v>-15</v>
+      </c>
+      <c r="D72">
+        <v>-15</v>
+      </c>
+      <c r="E72">
+        <v>-15</v>
+      </c>
+      <c r="F72">
+        <v>-15</v>
+      </c>
+      <c r="G72">
+        <v>-15</v>
+      </c>
+      <c r="H72">
+        <v>-15</v>
+      </c>
+      <c r="I72">
+        <v>15</v>
+      </c>
+      <c r="J72">
+        <v>-15</v>
+      </c>
+      <c r="K72">
+        <v>-15</v>
+      </c>
+      <c r="L72">
+        <v>-15</v>
+      </c>
+      <c r="M72">
+        <v>-15</v>
+      </c>
+      <c r="N72">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B73">
+        <v>-15</v>
+      </c>
+      <c r="C73">
+        <v>-15</v>
+      </c>
+      <c r="D73">
+        <v>-15</v>
+      </c>
+      <c r="E73">
+        <v>-15</v>
+      </c>
+      <c r="F73">
+        <v>15</v>
+      </c>
+      <c r="G73">
+        <v>-15</v>
+      </c>
+      <c r="H73">
+        <v>-15</v>
+      </c>
+      <c r="I73">
+        <v>-15</v>
+      </c>
+      <c r="J73">
+        <v>-15</v>
+      </c>
+      <c r="K73">
+        <v>-15</v>
+      </c>
+      <c r="L73">
+        <v>-15</v>
+      </c>
+      <c r="M73">
+        <v>-15</v>
+      </c>
+      <c r="N73">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B74">
+        <v>-15</v>
+      </c>
+      <c r="C74">
+        <v>-15</v>
+      </c>
+      <c r="D74">
+        <v>-15</v>
+      </c>
+      <c r="E74">
+        <v>-15</v>
+      </c>
+      <c r="F74">
+        <v>-15</v>
+      </c>
+      <c r="G74">
+        <v>-15</v>
+      </c>
+      <c r="H74">
+        <v>-15</v>
+      </c>
+      <c r="I74">
+        <v>15</v>
+      </c>
+      <c r="J74">
+        <v>-15</v>
+      </c>
+      <c r="K74">
+        <v>-15</v>
+      </c>
+      <c r="L74">
+        <v>-15</v>
+      </c>
+      <c r="M74">
+        <v>-15</v>
+      </c>
+      <c r="N74">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B75">
+        <v>-15</v>
+      </c>
+      <c r="C75">
+        <v>-15</v>
+      </c>
+      <c r="D75">
+        <v>15</v>
+      </c>
+      <c r="E75">
+        <v>-15</v>
+      </c>
+      <c r="F75">
+        <v>-15</v>
+      </c>
+      <c r="G75">
+        <v>-15</v>
+      </c>
+      <c r="H75">
+        <v>-15</v>
+      </c>
+      <c r="I75">
+        <v>-15</v>
+      </c>
+      <c r="J75">
+        <v>-15</v>
+      </c>
+      <c r="K75">
+        <v>-15</v>
+      </c>
+      <c r="L75">
+        <v>-15</v>
+      </c>
+      <c r="M75">
+        <v>-15</v>
+      </c>
+      <c r="N75">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="76" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B76">
+        <v>-15</v>
+      </c>
+      <c r="C76">
+        <v>-15</v>
+      </c>
+      <c r="D76">
+        <v>-15</v>
+      </c>
+      <c r="E76">
+        <v>-15</v>
+      </c>
+      <c r="F76">
+        <v>-15</v>
+      </c>
+      <c r="G76">
+        <v>-15</v>
+      </c>
+      <c r="H76">
+        <v>-15</v>
+      </c>
+      <c r="I76">
+        <v>15</v>
+      </c>
+      <c r="J76">
+        <v>-15</v>
+      </c>
+      <c r="K76">
+        <v>-15</v>
+      </c>
+      <c r="L76">
+        <v>-15</v>
+      </c>
+      <c r="M76">
+        <v>-15</v>
+      </c>
+      <c r="N76">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="77" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B77">
+        <v>-15</v>
+      </c>
+      <c r="C77">
+        <v>-15</v>
+      </c>
+      <c r="D77">
+        <v>15</v>
+      </c>
+      <c r="E77">
+        <v>-15</v>
+      </c>
+      <c r="F77">
+        <v>-15</v>
+      </c>
+      <c r="G77">
+        <v>-15</v>
+      </c>
+      <c r="H77">
+        <v>-15</v>
+      </c>
+      <c r="I77">
+        <v>-15</v>
+      </c>
+      <c r="J77">
+        <v>-15</v>
+      </c>
+      <c r="K77">
+        <v>-15</v>
+      </c>
+      <c r="L77">
+        <v>-15</v>
+      </c>
+      <c r="M77">
+        <v>-15</v>
+      </c>
+      <c r="N77">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="78" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B78">
+        <v>-15</v>
+      </c>
+      <c r="C78">
+        <v>-15</v>
+      </c>
+      <c r="D78">
+        <v>-15</v>
+      </c>
+      <c r="E78">
+        <v>-15</v>
+      </c>
+      <c r="F78">
+        <v>-15</v>
+      </c>
+      <c r="G78">
+        <v>-15</v>
+      </c>
+      <c r="H78">
+        <v>-15</v>
+      </c>
+      <c r="I78">
+        <v>15</v>
+      </c>
+      <c r="J78">
+        <v>-15</v>
+      </c>
+      <c r="K78">
+        <v>-15</v>
+      </c>
+      <c r="L78">
+        <v>-15</v>
+      </c>
+      <c r="M78">
+        <v>-15</v>
+      </c>
+      <c r="N78">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="79" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B79">
+        <v>-15</v>
+      </c>
+      <c r="C79">
+        <v>-15</v>
+      </c>
+      <c r="D79">
+        <v>15</v>
+      </c>
+      <c r="E79">
+        <v>-15</v>
+      </c>
+      <c r="F79">
+        <v>-15</v>
+      </c>
+      <c r="G79">
+        <v>-15</v>
+      </c>
+      <c r="H79">
+        <v>-15</v>
+      </c>
+      <c r="I79">
+        <v>-15</v>
+      </c>
+      <c r="J79">
+        <v>-15</v>
+      </c>
+      <c r="K79">
+        <v>-15</v>
+      </c>
+      <c r="L79">
+        <v>-15</v>
+      </c>
+      <c r="M79">
+        <v>-15</v>
+      </c>
+      <c r="N79">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="80" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B80">
+        <v>-15</v>
+      </c>
+      <c r="C80">
+        <v>-15</v>
+      </c>
+      <c r="D80">
+        <v>-15</v>
+      </c>
+      <c r="E80">
+        <v>-15</v>
+      </c>
+      <c r="F80">
+        <v>-15</v>
+      </c>
+      <c r="G80">
+        <v>-15</v>
+      </c>
+      <c r="H80">
+        <v>-15</v>
+      </c>
+      <c r="I80">
+        <v>15</v>
+      </c>
+      <c r="J80">
+        <v>-15</v>
+      </c>
+      <c r="K80">
+        <v>-15</v>
+      </c>
+      <c r="L80">
+        <v>-15</v>
+      </c>
+      <c r="M80">
+        <v>-15</v>
+      </c>
+      <c r="N80">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="81" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B81">
+        <v>-15</v>
+      </c>
+      <c r="C81">
+        <v>-15</v>
+      </c>
+      <c r="D81">
+        <v>15</v>
+      </c>
+      <c r="E81">
+        <v>-15</v>
+      </c>
+      <c r="F81">
+        <v>-15</v>
+      </c>
+      <c r="G81">
+        <v>-15</v>
+      </c>
+      <c r="H81">
+        <v>-15</v>
+      </c>
+      <c r="I81">
+        <v>-15</v>
+      </c>
+      <c r="J81">
+        <v>-15</v>
+      </c>
+      <c r="K81">
+        <v>-15</v>
+      </c>
+      <c r="L81">
+        <v>-15</v>
+      </c>
+      <c r="M81">
+        <v>-15</v>
+      </c>
+      <c r="N81">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="82" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B82">
+        <v>-15</v>
+      </c>
+      <c r="C82">
+        <v>-15</v>
+      </c>
+      <c r="D82">
+        <v>-15</v>
+      </c>
+      <c r="E82">
+        <v>-15</v>
+      </c>
+      <c r="F82">
+        <v>-15</v>
+      </c>
+      <c r="G82">
+        <v>-15</v>
+      </c>
+      <c r="H82">
+        <v>-15</v>
+      </c>
+      <c r="I82">
+        <v>15</v>
+      </c>
+      <c r="J82">
+        <v>-15</v>
+      </c>
+      <c r="K82">
+        <v>-15</v>
+      </c>
+      <c r="L82">
+        <v>-15</v>
+      </c>
+      <c r="M82">
+        <v>-15</v>
+      </c>
+      <c r="N82">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="83" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B83">
+        <v>10</v>
+      </c>
+      <c r="C83">
+        <v>-10</v>
+      </c>
+      <c r="D83">
+        <v>-10</v>
+      </c>
+      <c r="E83">
+        <v>-10</v>
+      </c>
+      <c r="F83">
+        <v>-10</v>
+      </c>
+      <c r="G83">
+        <v>-10</v>
+      </c>
+      <c r="H83">
+        <v>-10</v>
+      </c>
+      <c r="I83">
+        <v>-10</v>
+      </c>
+      <c r="J83">
+        <v>-10</v>
+      </c>
+      <c r="K83">
+        <v>-10</v>
+      </c>
+      <c r="L83">
+        <v>-10</v>
+      </c>
+      <c r="M83">
+        <v>-10</v>
+      </c>
+      <c r="N83">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="84" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B84">
+        <v>-5</v>
+      </c>
+      <c r="C84">
+        <v>-5</v>
+      </c>
+      <c r="D84">
+        <v>-5</v>
+      </c>
+      <c r="E84">
+        <v>-5</v>
+      </c>
+      <c r="F84">
+        <v>-5</v>
+      </c>
+      <c r="G84">
+        <v>-5</v>
+      </c>
+      <c r="H84">
+        <v>-5</v>
+      </c>
+      <c r="I84">
+        <v>-5</v>
+      </c>
+      <c r="J84">
+        <v>-5</v>
+      </c>
+      <c r="K84">
+        <v>-5</v>
+      </c>
+      <c r="L84">
+        <v>-5</v>
+      </c>
+      <c r="M84">
+        <v>-5</v>
+      </c>
+      <c r="N84">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="85" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B85">
+        <v>10</v>
+      </c>
+      <c r="C85">
+        <v>-10</v>
+      </c>
+      <c r="D85">
+        <v>-10</v>
+      </c>
+      <c r="E85">
+        <v>-10</v>
+      </c>
+      <c r="F85">
+        <v>-10</v>
+      </c>
+      <c r="G85">
+        <v>-10</v>
+      </c>
+      <c r="H85">
+        <v>-10</v>
+      </c>
+      <c r="I85">
+        <v>-10</v>
+      </c>
+      <c r="J85">
+        <v>-10</v>
+      </c>
+      <c r="K85">
+        <v>-10</v>
+      </c>
+      <c r="L85">
+        <v>-10</v>
+      </c>
+      <c r="M85">
+        <v>-10</v>
+      </c>
+      <c r="N85">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="86" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B86">
+        <v>-5</v>
+      </c>
+      <c r="C86">
+        <v>-5</v>
+      </c>
+      <c r="D86">
+        <v>-5</v>
+      </c>
+      <c r="E86">
+        <v>-5</v>
+      </c>
+      <c r="F86">
+        <v>-5</v>
+      </c>
+      <c r="G86">
+        <v>-5</v>
+      </c>
+      <c r="H86">
+        <v>-5</v>
+      </c>
+      <c r="I86">
+        <v>-5</v>
+      </c>
+      <c r="J86">
+        <v>-5</v>
+      </c>
+      <c r="K86">
+        <v>-5</v>
+      </c>
+      <c r="L86">
+        <v>-5</v>
+      </c>
+      <c r="M86">
+        <v>-5</v>
+      </c>
+      <c r="N86">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="87" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B87">
+        <v>30</v>
+      </c>
+      <c r="C87">
+        <v>-30</v>
+      </c>
+      <c r="D87">
+        <v>-30</v>
+      </c>
+      <c r="E87">
+        <v>-30</v>
+      </c>
+      <c r="F87">
+        <v>-30</v>
+      </c>
+      <c r="G87">
+        <v>-30</v>
+      </c>
+      <c r="H87">
+        <v>-30</v>
+      </c>
+      <c r="I87">
+        <v>-30</v>
+      </c>
+      <c r="J87">
+        <v>-30</v>
+      </c>
+      <c r="K87">
+        <v>-30</v>
+      </c>
+      <c r="L87">
+        <v>-30</v>
+      </c>
+      <c r="M87">
+        <v>-30</v>
+      </c>
+      <c r="N87">
+        <v>-30</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:N42">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="H59:H73">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:N58 I59:N73 B59:G73 B74:N87">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:N87">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>